<commit_message>
Added normalized counts per Grant's request
</commit_message>
<xml_diff>
--- a/MDA-MB-231-Cell-Count-Data/GH1909_1000nM_working_mod_8_22.xlsx
+++ b/MDA-MB-231-Cell-Count-Data/GH1909_1000nM_working_mod_8_22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grh57\Documents\MATLAB\2020 Incucyte Data Cal-Val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grh57\Desktop\Cell Count Data (Final MATLAB Format) v2\231\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,7 +339,7 @@
   <dimension ref="A1:G213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B1" sqref="B1:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -353,22 +349,22 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1921</v>
+        <v>1609.105180327869</v>
       </c>
       <c r="C1">
-        <v>1916</v>
+        <v>1711.8143015521064</v>
       </c>
       <c r="D1">
-        <v>1750</v>
+        <v>1483.1827309236949</v>
       </c>
       <c r="E1">
-        <v>2096</v>
+        <v>1852.7306873669716</v>
       </c>
       <c r="F1">
-        <v>2041</v>
+        <v>1737.7751312071055</v>
       </c>
       <c r="G1">
-        <v>2010</v>
+        <v>1735.2635869565217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -376,22 +372,22 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2054</v>
+        <v>1720.5112131147541</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>1804.7311529933479</v>
       </c>
       <c r="D2">
-        <v>1763</v>
+        <v>1494.2006597819852</v>
       </c>
       <c r="E2">
-        <v>2165</v>
+        <v>1913.7222987354453</v>
       </c>
       <c r="F2">
-        <v>2071</v>
+        <v>1763.3181267662496</v>
       </c>
       <c r="G2">
-        <v>1959</v>
+        <v>1691.2345108695654</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -399,22 +395,22 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>2107</v>
+        <v>1764.906098360656</v>
       </c>
       <c r="C3">
-        <v>2054</v>
+        <v>1835.1078159645231</v>
       </c>
       <c r="D3">
-        <v>1846</v>
+        <v>1564.5458978772233</v>
       </c>
       <c r="E3">
-        <v>2207</v>
+        <v>1950.8476273945164</v>
       </c>
       <c r="F3">
-        <v>2076</v>
+        <v>1767.5752926927737</v>
       </c>
       <c r="G3">
-        <v>2031</v>
+        <v>1753.3932065217393</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -422,22 +418,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>2222</v>
+        <v>1861.2346229508198</v>
       </c>
       <c r="C4">
-        <v>2046</v>
+        <v>1827.9603658536585</v>
       </c>
       <c r="D4">
-        <v>1907</v>
+        <v>1616.2454102122776</v>
       </c>
       <c r="E4">
-        <v>2257</v>
+        <v>1995.0444472267438</v>
       </c>
       <c r="F4">
-        <v>2186</v>
+        <v>1861.232943076302</v>
       </c>
       <c r="G4">
-        <v>2130</v>
+        <v>1838.8614130434785</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -445,22 +441,22 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>2278</v>
+        <v>1908.1424262295084</v>
       </c>
       <c r="C5">
-        <v>2138</v>
+        <v>1910.1560421286028</v>
       </c>
       <c r="D5">
-        <v>1982</v>
+        <v>1679.8103843947217</v>
       </c>
       <c r="E5">
-        <v>2370</v>
+        <v>2094.9292600475778</v>
       </c>
       <c r="F5">
-        <v>2216</v>
+        <v>1886.7759386354462</v>
       </c>
       <c r="G5">
-        <v>2183</v>
+        <v>1884.6171195652175</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -468,22 +464,22 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>2374</v>
+        <v>1988.5558032786887</v>
       </c>
       <c r="C6">
-        <v>2245</v>
+        <v>2005.7531873614189</v>
       </c>
       <c r="D6">
-        <v>2095</v>
+        <v>1775.5816121629375</v>
       </c>
       <c r="E6">
-        <v>2480</v>
+        <v>2192.1622636784778</v>
       </c>
       <c r="F6">
-        <v>2326</v>
+        <v>1980.4335890189748</v>
       </c>
       <c r="G6">
-        <v>2283</v>
+        <v>1970.948641304348</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -491,22 +487,22 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>2503</v>
+        <v>2096.6112786885246</v>
       </c>
       <c r="C7">
-        <v>2335</v>
+        <v>2086.1620011086475</v>
       </c>
       <c r="D7">
-        <v>2153</v>
+        <v>1824.7385255306942</v>
       </c>
       <c r="E7">
-        <v>2589</v>
+        <v>2288.5113309127337</v>
       </c>
       <c r="F7">
-        <v>2392</v>
+        <v>2036.6281792490918</v>
       </c>
       <c r="G7">
-        <v>2412</v>
+        <v>2082.3163043478262</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -514,22 +510,22 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>2627</v>
+        <v>2200.4785573770496</v>
       </c>
       <c r="C8">
-        <v>2429</v>
+        <v>2170.1445399113081</v>
       </c>
       <c r="D8">
-        <v>2246</v>
+        <v>1903.559093516925</v>
       </c>
       <c r="E8">
-        <v>2669</v>
+        <v>2359.2262426442971</v>
       </c>
       <c r="F8">
-        <v>2521</v>
+        <v>2146.4630601534113</v>
       </c>
       <c r="G8">
-        <v>2460</v>
+        <v>2123.755434782609</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -537,22 +533,22 @@
         <v>24</v>
       </c>
       <c r="B9">
-        <v>2699</v>
+        <v>2260.7885901639347</v>
       </c>
       <c r="C9">
-        <v>2485</v>
+        <v>2220.1766906873613</v>
       </c>
       <c r="D9">
-        <v>2364</v>
+        <v>2003.567986230637</v>
       </c>
       <c r="E9">
-        <v>2834</v>
+        <v>2505.0757480906477</v>
       </c>
       <c r="F9">
-        <v>2615</v>
+        <v>2226.4977795720633</v>
       </c>
       <c r="G9">
-        <v>2552</v>
+        <v>2203.1804347826087</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -560,22 +556,22 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <v>2813</v>
+        <v>2356.2794754098363</v>
       </c>
       <c r="C10">
-        <v>2661</v>
+        <v>2377.4205931263855</v>
       </c>
       <c r="D10">
-        <v>2495</v>
+        <v>2114.594807802639</v>
       </c>
       <c r="E10">
-        <v>2935</v>
+        <v>2594.3533241517471</v>
       </c>
       <c r="F10">
-        <v>2729</v>
+        <v>2323.5611626968107</v>
       </c>
       <c r="G10">
-        <v>2700</v>
+        <v>2330.951086956522</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -583,22 +579,22 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>3126</v>
+        <v>2618.4605901639347</v>
       </c>
       <c r="C11">
-        <v>2920</v>
+        <v>2608.8192904656316</v>
       </c>
       <c r="D11">
-        <v>2718</v>
+        <v>2303.594664371773</v>
       </c>
       <c r="E11">
-        <v>3239</v>
+        <v>2863.0699887316896</v>
       </c>
       <c r="F11">
-        <v>3000</v>
+        <v>2554.2995559144128</v>
       </c>
       <c r="G11">
-        <v>2933</v>
+        <v>2532.1035326086958</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -606,22 +602,22 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>3247</v>
+        <v>2719.8149508196725</v>
       </c>
       <c r="C12">
-        <v>3049</v>
+        <v>2724.0719235033257</v>
       </c>
       <c r="D12">
-        <v>2904</v>
+        <v>2461.2358003442341</v>
       </c>
       <c r="E12">
-        <v>3435</v>
+        <v>3036.3215224740206</v>
       </c>
       <c r="F12">
-        <v>3129</v>
+        <v>2664.1344368187324</v>
       </c>
       <c r="G12">
-        <v>3064</v>
+        <v>2645.1978260869569</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -629,22 +625,22 @@
         <v>36</v>
       </c>
       <c r="B13">
-        <v>3471</v>
+        <v>2907.4461639344263</v>
       </c>
       <c r="C13">
-        <v>3224</v>
+        <v>2880.4223946784919</v>
       </c>
       <c r="D13">
-        <v>3056</v>
+        <v>2590.060814687321</v>
       </c>
       <c r="E13">
-        <v>3617</v>
+        <v>3197.1979466633284</v>
       </c>
       <c r="F13">
-        <v>3333</v>
+        <v>2837.8268066209125</v>
       </c>
       <c r="G13">
-        <v>3281</v>
+        <v>2832.5372282608696</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -652,22 +648,22 @@
         <v>39</v>
       </c>
       <c r="B14">
-        <v>3699</v>
+        <v>3098.42793442623</v>
       </c>
       <c r="C14">
-        <v>3444</v>
+        <v>3076.9772727272725</v>
       </c>
       <c r="D14">
-        <v>3278</v>
+        <v>2778.2131382673551</v>
       </c>
       <c r="E14">
-        <v>3854</v>
+        <v>3406.6908726680863</v>
       </c>
       <c r="F14">
-        <v>3538</v>
+        <v>3012.3706096083974</v>
       </c>
       <c r="G14">
-        <v>3545</v>
+        <v>3060.452445652174</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -675,22 +671,22 @@
         <v>42</v>
       </c>
       <c r="B15">
-        <v>3867</v>
+        <v>3239.1513442622954</v>
       </c>
       <c r="C15">
-        <v>3699</v>
+        <v>3304.8022450110861</v>
       </c>
       <c r="D15">
-        <v>3438</v>
+        <v>2913.818416523236</v>
       </c>
       <c r="E15">
-        <v>3970</v>
+        <v>3509.2274946788539</v>
       </c>
       <c r="F15">
-        <v>3751</v>
+        <v>3193.7258780783209</v>
       </c>
       <c r="G15">
-        <v>3718</v>
+        <v>3209.8059782608698</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -698,22 +694,22 @@
         <v>44.966666666666697</v>
       </c>
       <c r="B16">
-        <v>3865</v>
+        <v>3237.4760655737709</v>
       </c>
       <c r="C16">
-        <v>3526</v>
+        <v>3150.238636363636</v>
       </c>
       <c r="D16">
-        <v>3463</v>
+        <v>2935.0067412507174</v>
       </c>
       <c r="E16">
-        <v>3979</v>
+        <v>3517.1829222486544</v>
       </c>
       <c r="F16">
-        <v>3792</v>
+        <v>3228.6346386758178</v>
       </c>
       <c r="G16">
-        <v>3668</v>
+        <v>3166.6402173913048</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -721,22 +717,22 @@
         <v>47.966666666666697</v>
       </c>
       <c r="B17">
-        <v>3914</v>
+        <v>3278.5203934426231</v>
       </c>
       <c r="C17">
-        <v>3719</v>
+        <v>3322.6708702882479</v>
       </c>
       <c r="D17">
-        <v>3569</v>
+        <v>3024.8452380952381</v>
       </c>
       <c r="E17">
-        <v>4112</v>
+        <v>3634.7464630023796</v>
       </c>
       <c r="F17">
-        <v>3833</v>
+        <v>3263.5433992733147</v>
       </c>
       <c r="G17">
-        <v>3767</v>
+        <v>3252.1084239130437</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -744,22 +740,22 @@
         <v>50.966666666666697</v>
       </c>
       <c r="B18">
-        <v>3892</v>
+        <v>3260.0923278688529</v>
       </c>
       <c r="C18">
-        <v>3677</v>
+        <v>3285.1467572062083</v>
       </c>
       <c r="D18">
-        <v>3537</v>
+        <v>2997.7241824440621</v>
       </c>
       <c r="E18">
-        <v>4068</v>
+        <v>3595.8532615500194</v>
       </c>
       <c r="F18">
-        <v>3789</v>
+        <v>3226.0803391199033</v>
       </c>
       <c r="G18">
-        <v>3714</v>
+        <v>3206.3527173913044</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -767,22 +763,22 @@
         <v>53.966666666666697</v>
       </c>
       <c r="B19">
-        <v>3964</v>
+        <v>3320.402360655738</v>
       </c>
       <c r="C19">
-        <v>3665</v>
+        <v>3274.4255820399112</v>
       </c>
       <c r="D19">
-        <v>3562</v>
+        <v>3018.9125071715434</v>
       </c>
       <c r="E19">
-        <v>4125</v>
+        <v>3646.2376361587585</v>
       </c>
       <c r="F19">
-        <v>3812</v>
+        <v>3245.663302381914</v>
       </c>
       <c r="G19">
-        <v>3748</v>
+        <v>3235.7054347826088</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -790,22 +786,22 @@
         <v>56.966666666666697</v>
       </c>
       <c r="B20">
-        <v>3907</v>
+        <v>3272.656918032787</v>
       </c>
       <c r="C20">
-        <v>3599</v>
+        <v>3215.4591186252769</v>
       </c>
       <c r="D20">
-        <v>3523</v>
+        <v>2985.8587205966724</v>
       </c>
       <c r="E20">
-        <v>4072</v>
+        <v>3599.3890071365977</v>
       </c>
       <c r="F20">
-        <v>3757</v>
+        <v>3198.8344771901498</v>
       </c>
       <c r="G20">
-        <v>3730</v>
+        <v>3220.1657608695655</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -813,22 +809,22 @@
         <v>59.966666666666697</v>
       </c>
       <c r="B21">
-        <v>3885</v>
+        <v>3254.2288524590167</v>
       </c>
       <c r="C21">
-        <v>3581</v>
+        <v>3199.3773558758312</v>
       </c>
       <c r="D21">
-        <v>3479</v>
+        <v>2948.5672690763054</v>
       </c>
       <c r="E21">
-        <v>4009</v>
+        <v>3543.7010141479909</v>
       </c>
       <c r="F21">
-        <v>3760</v>
+        <v>3201.3887767460642</v>
       </c>
       <c r="G21">
-        <v>3659</v>
+        <v>3158.8703804347829</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -836,22 +832,22 @@
         <v>62.966666666666697</v>
       </c>
       <c r="B22">
-        <v>3844</v>
+        <v>3219.8856393442625</v>
       </c>
       <c r="C22">
-        <v>3644</v>
+        <v>3255.663525498891</v>
       </c>
       <c r="D22">
-        <v>3459</v>
+        <v>2931.6166092943204</v>
       </c>
       <c r="E22">
-        <v>3977</v>
+        <v>3515.4150494553655</v>
       </c>
       <c r="F22">
-        <v>3717</v>
+        <v>3164.7771497779572</v>
       </c>
       <c r="G22">
-        <v>3632</v>
+        <v>3135.5608695652177</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -859,22 +855,22 @@
         <v>65.966666666666697</v>
       </c>
       <c r="B23">
-        <v>3823</v>
+        <v>3202.2952131147545</v>
       </c>
       <c r="C23">
-        <v>3620</v>
+        <v>3234.2211751662967</v>
       </c>
       <c r="D23">
-        <v>3477</v>
+        <v>2946.8722030981066</v>
       </c>
       <c r="E23">
-        <v>3988</v>
+        <v>3525.1383498184555</v>
       </c>
       <c r="F23">
-        <v>3716</v>
+        <v>3163.9257165926529</v>
       </c>
       <c r="G23">
-        <v>3664</v>
+        <v>3163.1869565217394</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>